<commit_message>
Print a rudimentary color-producing ally
</commit_message>
<xml_diff>
--- a/data/allies/resource_allies.xlsx
+++ b/data/allies/resource_allies.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Red Ally</t>
   </si>
   <si>
-    <t xml:space="preserve">1R1Y</t>
+    <t xml:space="preserve">2R1Y</t>
   </si>
   <si>
     <t xml:space="preserve">R</t>
@@ -200,7 +200,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>